<commit_message>
Remoção do buzzer no Cronometro
</commit_message>
<xml_diff>
--- a/Docs/Queda_Livre.xlsx
+++ b/Docs/Queda_Livre.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>S entre sensores(mm)</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>Aceleração</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Média</t>
   </si>
 </sst>
 </file>
@@ -509,10 +515,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="J2" sqref="J2:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -521,7 +527,7 @@
     <col min="6" max="6" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:11">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -540,89 +546,152 @@
       <c r="F1" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="5">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="B2" s="5">
-        <v>200</v>
+        <f>A2</f>
+        <v>220</v>
       </c>
       <c r="C2" s="5">
         <v>0.2</v>
       </c>
       <c r="D2" s="9">
-        <v>178</v>
+        <v>210</v>
       </c>
       <c r="E2" s="7">
-        <v>0.17799999999999999</v>
+        <f>D2/1000</f>
+        <v>0.21</v>
       </c>
       <c r="F2" s="6">
-        <v>12.624668602449187</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <f>2*C2/(E2^2)</f>
+        <v>9.0702947845805006</v>
+      </c>
+      <c r="H2">
+        <f>(9.8*E2^2)/2</f>
+        <v>0.21608999999999998</v>
+      </c>
+      <c r="I2">
+        <f>H2*1000</f>
+        <v>216.08999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="5">
         <v>185</v>
       </c>
       <c r="B3" s="5">
-        <v>385</v>
+        <f>B2+A3</f>
+        <v>405</v>
       </c>
       <c r="C3" s="5">
         <v>0.38500000000000001</v>
       </c>
       <c r="D3" s="9">
-        <v>259</v>
+        <v>285</v>
       </c>
       <c r="E3" s="7">
-        <v>0.25900000000000001</v>
+        <f t="shared" ref="E3:E5" si="0">D3/1000</f>
+        <v>0.28499999999999998</v>
       </c>
       <c r="F3" s="6">
-        <v>11.478660127308776</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <f>2*C3/(E3^2)</f>
+        <v>9.47983995075408</v>
+      </c>
+      <c r="H3" s="4">
+        <f t="shared" ref="H3:H5" si="1">(9.8*E3^2)/2</f>
+        <v>0.39800249999999998</v>
+      </c>
+      <c r="I3" s="4">
+        <f t="shared" ref="I3:I5" si="2">H3*1000</f>
+        <v>398.0025</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="5">
         <v>200</v>
       </c>
       <c r="B4" s="5">
-        <v>585</v>
+        <f t="shared" ref="B4:B5" si="3">B3+A4</f>
+        <v>605</v>
       </c>
       <c r="C4" s="5">
         <v>0.58499999999999996</v>
       </c>
       <c r="D4" s="9">
-        <v>329</v>
+        <v>352</v>
       </c>
       <c r="E4" s="7">
-        <v>0.32900000000000001</v>
+        <f t="shared" si="0"/>
+        <v>0.35199999999999998</v>
       </c>
       <c r="F4" s="6">
-        <v>10.809212775196089</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <f t="shared" ref="F3:F5" si="4">2*C4/(E4^2)</f>
+        <v>9.4427944214876032</v>
+      </c>
+      <c r="H4" s="4">
+        <f t="shared" si="1"/>
+        <v>0.60712959999999994</v>
+      </c>
+      <c r="I4" s="4">
+        <f t="shared" si="2"/>
+        <v>607.12959999999998</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="5">
         <v>195</v>
       </c>
       <c r="B5" s="5">
-        <v>780</v>
+        <f t="shared" si="3"/>
+        <v>800</v>
       </c>
       <c r="C5" s="5">
         <v>0.78</v>
       </c>
       <c r="D5" s="9">
-        <v>383</v>
+        <v>403</v>
       </c>
       <c r="E5" s="7">
-        <v>0.38300000000000001</v>
+        <f t="shared" si="0"/>
+        <v>0.40300000000000002</v>
       </c>
       <c r="F5" s="6">
-        <v>10.634744254852102</v>
+        <f t="shared" si="4"/>
+        <v>9.605379012246857</v>
+      </c>
+      <c r="H5" s="4">
+        <f t="shared" si="1"/>
+        <v>0.79580410000000024</v>
+      </c>
+      <c r="I5" s="4">
+        <f t="shared" si="2"/>
+        <v>795.80410000000029</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="E7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="6">
+        <f>AVERAGE(F2:F5)</f>
+        <v>9.3995770422672607</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Alterações no codigo Queda Livre
</commit_message>
<xml_diff>
--- a/Docs/Queda_Livre.xlsx
+++ b/Docs/Queda_Livre.xlsx
@@ -518,7 +518,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:K7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -552,33 +552,34 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B2" s="5">
         <f>A2</f>
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C2" s="5">
-        <v>0.2</v>
+        <f>B2/1000</f>
+        <v>0.222</v>
       </c>
       <c r="D2" s="9">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E2" s="7">
         <f>D2/1000</f>
-        <v>0.21</v>
+        <v>0.21199999999999999</v>
       </c>
       <c r="F2" s="6">
         <f>2*C2/(E2^2)</f>
-        <v>9.0702947845805006</v>
+        <v>9.878960484158064</v>
       </c>
       <c r="H2">
         <f>(9.8*E2^2)/2</f>
-        <v>0.21608999999999998</v>
+        <v>0.22022559999999999</v>
       </c>
       <c r="I2">
         <f>H2*1000</f>
-        <v>216.08999999999997</v>
+        <v>220.22559999999999</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -587,29 +588,29 @@
       </c>
       <c r="B3" s="5">
         <f>B2+A3</f>
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="C3" s="5">
         <v>0.38500000000000001</v>
       </c>
       <c r="D3" s="9">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="E3" s="7">
         <f t="shared" ref="E3:E5" si="0">D3/1000</f>
-        <v>0.28499999999999998</v>
+        <v>0.28799999999999998</v>
       </c>
       <c r="F3" s="6">
         <f>2*C3/(E3^2)</f>
-        <v>9.47983995075408</v>
+        <v>9.2833719135802486</v>
       </c>
       <c r="H3" s="4">
         <f t="shared" ref="H3:H5" si="1">(9.8*E3^2)/2</f>
-        <v>0.39800249999999998</v>
+        <v>0.4064256</v>
       </c>
       <c r="I3" s="4">
         <f t="shared" ref="I3:I5" si="2">H3*1000</f>
-        <v>398.0025</v>
+        <v>406.42559999999997</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -620,29 +621,29 @@
       </c>
       <c r="B4" s="5">
         <f t="shared" ref="B4:B5" si="3">B3+A4</f>
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="C4" s="5">
         <v>0.58499999999999996</v>
       </c>
       <c r="D4" s="9">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="E4" s="7">
         <f t="shared" si="0"/>
-        <v>0.35199999999999998</v>
+        <v>0.35399999999999998</v>
       </c>
       <c r="F4" s="6">
-        <f t="shared" ref="F3:F5" si="4">2*C4/(E4^2)</f>
-        <v>9.4427944214876032</v>
+        <f t="shared" ref="F4:F5" si="4">2*C4/(E4^2)</f>
+        <v>9.3363975869003166</v>
       </c>
       <c r="H4" s="4">
         <f t="shared" si="1"/>
-        <v>0.60712959999999994</v>
+        <v>0.61404839999999994</v>
       </c>
       <c r="I4" s="4">
         <f t="shared" si="2"/>
-        <v>607.12959999999998</v>
+        <v>614.0483999999999</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -653,29 +654,29 @@
       </c>
       <c r="B5" s="5">
         <f t="shared" si="3"/>
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="C5" s="5">
         <v>0.78</v>
       </c>
       <c r="D5" s="9">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="E5" s="7">
         <f t="shared" si="0"/>
-        <v>0.40300000000000002</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="F5" s="6">
         <f t="shared" si="4"/>
-        <v>9.605379012246857</v>
+        <v>9.5107453132144482</v>
       </c>
       <c r="H5" s="4">
         <f t="shared" si="1"/>
-        <v>0.79580410000000024</v>
+        <v>0.80372250000000023</v>
       </c>
       <c r="I5" s="4">
         <f t="shared" si="2"/>
-        <v>795.80410000000029</v>
+        <v>803.7225000000002</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
@@ -686,7 +687,7 @@
       </c>
       <c r="F7" s="6">
         <f>AVERAGE(F2:F5)</f>
-        <v>9.3995770422672607</v>
+        <v>9.5023688244632698</v>
       </c>
     </row>
   </sheetData>

</xml_diff>